<commit_message>
add OTree derived  classes
</commit_message>
<xml_diff>
--- a/jsonData.xlsx
+++ b/jsonData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\[unityprojects\Fish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB0734F-2C0B-4A78-85F5-C7955659551D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ACF4AE-2D79-44BC-9A92-849D4AD20ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -373,10 +373,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>电鲶，为辐鳍鱼纲鲶形目电鲶科的其中一种，分布于非洲尼罗河、查德湖、尼日河、塞内加尔河、图尔卡纳湖等流域，体长可达122公分，生活在岩石、树根沉积的底中层水域，在夜间活动，属肉食性，具有发电器官，以电击击昏猎物，可做为食用鱼、游钓鱼及观赏鱼。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>电鲶</t>
   </si>
   <si>
@@ -422,10 +418,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>白斑狗鱼，为辐鳍鱼纲狗鱼目狗鱼科的其中一种。分布于北美洲及欧亚大陆74°N-36°N的淡水流域，体长可达137公分，主要栖息在有植被生长的泠水湖泊、河川，属肉食性，以鱼类、甲壳类、鸟类、小型哺乳类等为食，可作为观赏鱼、游钓鱼及食用鱼，适合各种烹饪方式食用。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>蝴蝶鱼俗称热带鱼，是近海暖水性小型珊瑚礁鱼类，体型最大的细纹蝴蝶鱼可达30多厘米。蝴蝶鱼身体侧扁，可以在珊瑚丛中敏捷地穿梭。大部分蝶鱼在眼睛上还有一条黑色纵带穿过，亦有将头部伪装以使欺敌之作用。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -451,6 +443,14 @@
   </si>
   <si>
     <t>石斑鱼属于辐鳍鱼纲，身体肥厚，口部大，并不适宜长途迅速游泳。石斑鱼的种类颇多，体型大小也各有差别。它们会把猎物吞噬，而不会用口把猎物逐片撕开；这是因为它们的颚没有很多牙齿，可是在咽头里的牙板可以碾碎食物。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电鲶，为辐鳍鱼纲鲶形目电鲶科的其中一种，分布于非洲尼罗河、查德湖、尼日河、塞内加尔河、图尔卡纳湖等流域，体长可达122公分，生活在岩石、树根沉积的底中层水域，在夜间活动，属肉食性，具有发电器官，以电击击昏猎物。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白斑狗鱼，为辐鳍鱼纲狗鱼目狗鱼科的其中一种。分布于北美洲及欧亚大陆74°N-36°N的淡水流域，体长可达137公分，主要栖息在有植被生长的泠水湖泊、河川，属肉食性，以鱼类、甲壳类、鸟类、小型哺乳类等为食，可作为观赏鱼、游钓鱼及食用鱼。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -788,7 +788,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -819,19 +819,19 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>93</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>94</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>95</v>
-      </c>
-      <c r="H1" t="s">
-        <v>96</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -896,7 +896,7 @@
         <v>81</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -937,13 +937,13 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M3" t="s">
         <v>80</v>
       </c>
       <c r="N3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O3">
         <v>2</v>
@@ -984,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M4" t="s">
         <v>45</v>
@@ -1034,10 +1034,10 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N5" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="O5">
         <v>4</v>
@@ -1084,7 +1084,7 @@
         <v>16</v>
       </c>
       <c r="N6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O6">
         <v>5</v>
@@ -1131,7 +1131,7 @@
         <v>30</v>
       </c>
       <c r="N7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O7">
         <v>6</v>
@@ -1292,7 +1292,7 @@
         <v>10</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F11">
         <v>8</v>
@@ -1413,7 +1413,7 @@
         <v>43</v>
       </c>
       <c r="N13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O13">
         <v>12</v>
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -1454,13 +1454,13 @@
         <v>1</v>
       </c>
       <c r="L14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M14" t="s">
         <v>44</v>
       </c>
       <c r="N14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O14">
         <v>13</v>
@@ -1524,10 +1524,10 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -1548,13 +1548,13 @@
         <v>1</v>
       </c>
       <c r="L16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M16" t="s">
         <v>49</v>
       </c>
       <c r="N16" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="O16">
         <v>15</v>
@@ -1742,7 +1742,7 @@
         <v>55</v>
       </c>
       <c r="N20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O20">
         <v>18</v>
@@ -1880,10 +1880,10 @@
         <v>1</v>
       </c>
       <c r="M23" t="s">
+        <v>89</v>
+      </c>
+      <c r="N23" t="s">
         <v>90</v>
-      </c>
-      <c r="N23" t="s">
-        <v>91</v>
       </c>
       <c r="O23">
         <v>20</v>
@@ -1927,10 +1927,10 @@
         <v>1</v>
       </c>
       <c r="M24" t="s">
+        <v>89</v>
+      </c>
+      <c r="N24" t="s">
         <v>90</v>
-      </c>
-      <c r="N24" t="s">
-        <v>91</v>
       </c>
       <c r="O24">
         <v>20</v>
@@ -2165,7 +2165,7 @@
         <v>66</v>
       </c>
       <c r="N29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O29">
         <v>24</v>

</xml_diff>